<commit_message>
Use improved tooth profile
</commit_message>
<xml_diff>
--- a/Belt specs.xlsx
+++ b/Belt specs.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\School\Waterloo\4A_F21\MTE481\q-pup-mechanical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501F8F8A-32F1-40AA-BF8C-34DACDD5FA9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D71C4B4-8939-4C11-A4BD-7AB133588852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A4784504-88B9-441C-AB45-7A22F78AE512}"/>
+    <workbookView xWindow="28680" yWindow="-15" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A4784504-88B9-441C-AB45-7A22F78AE512}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Pulley Design" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>power [kW]</t>
   </si>
@@ -64,13 +65,77 @@
   </si>
   <si>
     <t>DELTA</t>
+  </si>
+  <si>
+    <t>Gates Powergrip Drive Design Manual</t>
+  </si>
+  <si>
+    <t>https://www.gates.com/content/dam/gates/home/knowledge-center/resource-library/catalogs/powergripdrivedesignmanual_17195_2014.pdf</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Pages</t>
+  </si>
+  <si>
+    <t>Technical Data Sheet - optibelt OMEGA HP 8M</t>
+  </si>
+  <si>
+    <t>https://www.optibelt.com/fileadmin/pdf/datenblaetter/Technical-Data-Sheet-optibelt-OMEGA-HP-8M.pdf</t>
+  </si>
+  <si>
+    <t>https://www.optibelt.com/fileadmin/pdf/produkte/zahnriemen-gummi/Optibelt-TM-Rubber-Timing-Belt-Drives.pdf</t>
+  </si>
+  <si>
+    <t>Optibelt-TM-Rubber-Timing-Belt-Drives</t>
+  </si>
+  <si>
+    <t>Teeth</t>
+  </si>
+  <si>
+    <t>[1]</t>
+  </si>
+  <si>
+    <t>[2]</t>
+  </si>
+  <si>
+    <t>[3]</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Pitch Dia</t>
+  </si>
+  <si>
+    <t>Outside Dia</t>
+  </si>
+  <si>
+    <t>Pitch Dia (Alt)</t>
+  </si>
+  <si>
+    <t>Outside Dia (Alt)</t>
+  </si>
+  <si>
+    <t>131, 138</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="5">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000000"/>
+    <numFmt numFmtId="167" formatCode="0.00000000"/>
+    <numFmt numFmtId="168" formatCode="0.0000000000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +147,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -104,10 +177,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -117,8 +191,15 @@
       <alignment textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -433,7 +514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F78F5228-216D-46DA-9BAF-D312C7CBD806}">
   <dimension ref="A2:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -517,14 +598,14 @@
         <v>2850</v>
       </c>
       <c r="D5" s="1">
-        <f>B5*1000*9.5488/C5</f>
+        <f t="shared" ref="D5:D15" si="0">B5*1000*9.5488/C5</f>
         <v>16.752280701754387</v>
       </c>
       <c r="E5" s="1">
         <v>76.39</v>
       </c>
       <c r="F5" s="1">
-        <f>D5/(E5/2000)</f>
+        <f t="shared" ref="F5:F15" si="1">D5/(E5/2000)</f>
         <v>438.59878784538256</v>
       </c>
       <c r="G5" s="1">
@@ -544,21 +625,21 @@
         <v>10</v>
       </c>
       <c r="D6" s="1">
-        <f>B6*1000*9.5488/C6</f>
+        <f t="shared" si="0"/>
         <v>95.488</v>
       </c>
       <c r="E6" s="1">
         <v>81.489999999999995</v>
       </c>
       <c r="F6" s="1">
-        <f>D6/(E6/2000)</f>
+        <f t="shared" si="1"/>
         <v>2343.5513559946007</v>
       </c>
       <c r="G6" s="1">
         <v>20</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" ref="I6" si="0">F6/G6</f>
+        <f t="shared" ref="I6" si="2">F6/G6</f>
         <v>117.17756779973004</v>
       </c>
     </row>
@@ -571,21 +652,21 @@
         <v>20</v>
       </c>
       <c r="D7" s="1">
-        <f>B7*1000*9.5488/C7</f>
+        <f t="shared" si="0"/>
         <v>90.7136</v>
       </c>
       <c r="E7" s="1">
         <v>81.489999999999995</v>
       </c>
       <c r="F7" s="1">
-        <f>D7/(E7/2000)</f>
+        <f t="shared" si="1"/>
         <v>2226.3737881948709</v>
       </c>
       <c r="G7" s="1">
         <v>20</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" ref="I7" si="1">F7/G7</f>
+        <f t="shared" ref="I7" si="3">F7/G7</f>
         <v>111.31868940974354</v>
       </c>
       <c r="K7">
@@ -603,21 +684,21 @@
         <v>30</v>
       </c>
       <c r="D8" s="1">
-        <f>B8*1000*9.5488/C8</f>
+        <f t="shared" si="0"/>
         <v>90.183111111111117</v>
       </c>
       <c r="E8" s="1">
         <v>81.489999999999995</v>
       </c>
       <c r="F8" s="1">
-        <f>D8/(E8/2000)</f>
+        <f t="shared" si="1"/>
         <v>2213.3540584393454</v>
       </c>
       <c r="G8" s="1">
         <v>20</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" ref="I8" si="2">F8/G8</f>
+        <f t="shared" ref="I8" si="4">F8/G8</f>
         <v>110.66770292196728</v>
       </c>
     </row>
@@ -630,21 +711,21 @@
         <v>50</v>
       </c>
       <c r="D9" s="1">
-        <f>B9*1000*9.5488/C9</f>
+        <f t="shared" si="0"/>
         <v>89.758719999999997</v>
       </c>
       <c r="E9" s="1">
         <v>81.489999999999995</v>
       </c>
       <c r="F9" s="1">
-        <f>D9/(E9/2000)</f>
+        <f t="shared" si="1"/>
         <v>2202.9382746349247</v>
       </c>
       <c r="G9" s="1">
         <v>20</v>
       </c>
       <c r="I9" s="1">
-        <f t="shared" ref="I9" si="3">F9/G9</f>
+        <f t="shared" ref="I9" si="5">F9/G9</f>
         <v>110.14691373174624</v>
       </c>
     </row>
@@ -657,21 +738,21 @@
         <v>200</v>
       </c>
       <c r="D10" s="1">
-        <f>B10*1000*9.5488/C10</f>
+        <f t="shared" si="0"/>
         <v>81.642240000000001</v>
       </c>
       <c r="E10" s="1">
         <v>81.489999999999995</v>
       </c>
       <c r="F10" s="1">
-        <f>D10/(E10/2000)</f>
+        <f t="shared" si="1"/>
         <v>2003.7364093753836</v>
       </c>
       <c r="G10" s="1">
         <v>20</v>
       </c>
       <c r="I10" s="1">
-        <f t="shared" ref="I10:I15" si="4">F10/G10</f>
+        <f t="shared" ref="I10:I15" si="6">F10/G10</f>
         <v>100.18682046876918</v>
       </c>
     </row>
@@ -684,21 +765,21 @@
         <v>3000</v>
       </c>
       <c r="D11" s="1">
-        <f>B11*1000*9.5488/C11</f>
+        <f t="shared" si="0"/>
         <v>63.658666666666669</v>
       </c>
       <c r="E11" s="1">
         <v>81.489999999999995</v>
       </c>
       <c r="F11" s="1">
-        <f>D11/(E11/2000)</f>
+        <f t="shared" si="1"/>
         <v>1562.3675706630672</v>
       </c>
       <c r="G11" s="1">
         <v>20</v>
       </c>
       <c r="I11" s="1">
-        <f t="shared" ref="I11" si="5">F11/G11</f>
+        <f t="shared" ref="I11" si="7">F11/G11</f>
         <v>78.118378533153361</v>
       </c>
     </row>
@@ -711,21 +792,21 @@
         <v>8000</v>
       </c>
       <c r="D12" s="1">
-        <f>B12*1000*9.5488/C12</f>
+        <f t="shared" si="0"/>
         <v>52.422911999999997</v>
       </c>
       <c r="E12" s="1">
         <v>81.489999999999995</v>
       </c>
       <c r="F12" s="1">
-        <f>D12/(E12/2000)</f>
+        <f t="shared" si="1"/>
         <v>1286.6096944410358</v>
       </c>
       <c r="G12" s="1">
         <v>20</v>
       </c>
       <c r="I12" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>64.330484722051793</v>
       </c>
     </row>
@@ -740,21 +821,21 @@
         <v>20</v>
       </c>
       <c r="D13" s="1">
-        <f>B13*1000*9.5488/C13</f>
+        <f t="shared" si="0"/>
         <v>105.0368</v>
       </c>
       <c r="E13" s="1">
         <v>81.489999999999995</v>
       </c>
       <c r="F13" s="1">
-        <f>D13/(E13/2000)</f>
+        <f t="shared" si="1"/>
         <v>2577.9064915940608</v>
       </c>
       <c r="G13" s="1">
         <v>12</v>
       </c>
       <c r="I13" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>214.82554096617173</v>
       </c>
     </row>
@@ -767,21 +848,21 @@
         <v>30</v>
       </c>
       <c r="D14" s="1">
-        <f>B14*1000*9.5488/C14</f>
+        <f t="shared" si="0"/>
         <v>100.2624</v>
       </c>
       <c r="E14" s="1">
         <v>81.489999999999995</v>
       </c>
       <c r="F14" s="1">
-        <f>D14/(E14/2000)</f>
+        <f t="shared" si="1"/>
         <v>2460.728923794331</v>
       </c>
       <c r="G14" s="1">
         <v>12</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>205.06074364952758</v>
       </c>
       <c r="K14">
@@ -801,21 +882,21 @@
         <v>40</v>
       </c>
       <c r="D15" s="1">
-        <f>B15*1000*9.5488/C15</f>
+        <f t="shared" si="0"/>
         <v>97.875199999999992</v>
       </c>
       <c r="E15" s="1">
         <v>81.489999999999995</v>
       </c>
       <c r="F15" s="1">
-        <f>D15/(E15/2000)</f>
+        <f t="shared" si="1"/>
         <v>2402.1401398944654</v>
       </c>
       <c r="G15" s="1">
         <v>12</v>
       </c>
       <c r="I15" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>200.17834499120545</v>
       </c>
     </row>
@@ -823,4 +904,212 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8859C009-024E-402F-8A14-66C368B4486E}">
+  <dimension ref="B1:T17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="32.88671875" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" customWidth="1"/>
+    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:20" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2">
+        <v>39</v>
+      </c>
+      <c r="L2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3">
+        <v>99.31</v>
+      </c>
+      <c r="L3">
+        <v>160.43</v>
+      </c>
+      <c r="M3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="4">
+        <v>56</v>
+      </c>
+      <c r="P3" s="7">
+        <v>5.6139999999999999</v>
+      </c>
+      <c r="Q3" s="7">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4">
+        <v>75</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4">
+        <v>97.94</v>
+      </c>
+      <c r="L4">
+        <v>159.06</v>
+      </c>
+      <c r="M4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" s="4">
+        <v>63</v>
+      </c>
+      <c r="P4" s="7">
+        <f>(P5-P3)/($O5-$O3)*($O4-$O3)+P3</f>
+        <v>6.3157500000000004</v>
+      </c>
+      <c r="Q4" s="7">
+        <f>(Q5-Q3)/($O5-$O3)*($O4-$O3)+Q3</f>
+        <v>6.2617500000000001</v>
+      </c>
+      <c r="S4" s="1">
+        <f>P4*25.4</f>
+        <v>160.42005</v>
+      </c>
+      <c r="T4" s="1">
+        <f>Q4*25.4</f>
+        <v>159.04845</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="J5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="1">
+        <f>3.91*25.4</f>
+        <v>99.313999999999993</v>
+      </c>
+      <c r="L5" s="1">
+        <f>S4</f>
+        <v>160.42005</v>
+      </c>
+      <c r="M5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O5" s="4">
+        <v>64</v>
+      </c>
+      <c r="P5" s="7">
+        <v>6.4160000000000004</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>6.3620000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="J6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="1">
+        <f>3.856*25.4</f>
+        <v>97.942399999999992</v>
+      </c>
+      <c r="L6" s="1">
+        <f>T4</f>
+        <v>159.04845</v>
+      </c>
+      <c r="M6" t="s">
+        <v>20</v>
+      </c>
+      <c r="O6" s="4"/>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="P11" s="6"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="O15" s="4"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="10"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="O16" s="4"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="9"/>
+    </row>
+    <row r="17" spans="15:18" x14ac:dyDescent="0.3">
+      <c r="O17" s="4"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="9"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{5E74E6FF-1C34-4461-AF69-291484E7C3D1}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{0276A500-9218-4286-B195-FF533AE50649}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{3C8ED58E-B5B9-4310-9AF3-1B58BCF2B1AF}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId4"/>
+</worksheet>
 </file>
</xml_diff>